<commit_message>
Updates survye template. Adds conditional validations to LoggedDay to accommodate non fishing days
</commit_message>
<xml_diff>
--- a/public/templates/SmallPelagicLandingSite.template.xlsx
+++ b/public/templates/SmallPelagicLandingSite.template.xlsx
@@ -2472,21 +2472,9 @@
     <t>Pantai Jasi</t>
   </si>
   <si>
-    <t xml:space="preserve">Banjar Pengalon </t>
-  </si>
-  <si>
     <t>Tanah Ampo</t>
   </si>
   <si>
-    <t xml:space="preserve">Bunutun </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seraya </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kusamba </t>
-  </si>
-  <si>
     <t>Candidasa</t>
   </si>
   <si>
@@ -2514,12 +2502,6 @@
     <t>No. vessels</t>
   </si>
   <si>
-    <t xml:space="preserve">Jemelut </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amed </t>
-  </si>
-  <si>
     <t>Angantelo</t>
   </si>
   <si>
@@ -2566,6 +2548,24 @@
   </si>
   <si>
     <t>Wave</t>
+  </si>
+  <si>
+    <t>Seraya</t>
+  </si>
+  <si>
+    <t>Amed</t>
+  </si>
+  <si>
+    <t>Banjar Pengalon</t>
+  </si>
+  <si>
+    <t>Bunutun</t>
+  </si>
+  <si>
+    <t>Jemelut</t>
+  </si>
+  <si>
+    <t>Kusamba</t>
   </si>
 </sst>
 </file>
@@ -3893,7 +3893,7 @@
     </row>
     <row r="6" spans="1:3" s="33" customFormat="1" ht="28" customHeight="1">
       <c r="A6" s="36" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="B6" s="52"/>
       <c r="C6" s="34"/>
@@ -4008,10 +4008,10 @@
         <v>34</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>832</v>
+        <v>826</v>
       </c>
       <c r="J1" s="20" t="s">
         <v>13</v>
@@ -4020,7 +4020,7 @@
         <v>15</v>
       </c>
       <c r="L1" s="20" t="s">
-        <v>834</v>
+        <v>828</v>
       </c>
       <c r="M1" s="20" t="s">
         <v>17</v>
@@ -4035,10 +4035,10 @@
         <v>23</v>
       </c>
       <c r="Q1" s="20" t="s">
-        <v>833</v>
+        <v>827</v>
       </c>
       <c r="R1" s="20" t="s">
-        <v>845</v>
+        <v>839</v>
       </c>
       <c r="S1" s="20" t="s">
         <v>805</v>
@@ -5543,7 +5543,7 @@
         <v>45</v>
       </c>
       <c r="B1" s="49" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>32</v>
@@ -5552,7 +5552,7 @@
         <v>34</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="F1" s="7"/>
     </row>
@@ -33905,52 +33905,52 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="30" t="s">
-        <v>835</v>
+        <v>829</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="30" t="s">
-        <v>836</v>
+        <v>830</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="30" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="30" t="s">
-        <v>838</v>
+        <v>832</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="30" t="s">
-        <v>839</v>
+        <v>833</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="30" t="s">
-        <v>840</v>
+        <v>834</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="30" t="s">
-        <v>841</v>
+        <v>835</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="30" t="s">
-        <v>842</v>
+        <v>836</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="30" t="s">
-        <v>843</v>
+        <v>837</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="30" t="s">
-        <v>844</v>
+        <v>838</v>
       </c>
     </row>
   </sheetData>
@@ -34018,7 +34018,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -34029,61 +34029,61 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="38" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="B1" s="43"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="44" t="s">
-        <v>829</v>
+        <v>841</v>
       </c>
       <c r="B2" s="7"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="44" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="B3" s="7"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="44" t="s">
-        <v>830</v>
+        <v>824</v>
       </c>
       <c r="B4" s="7"/>
     </row>
     <row r="5" spans="1:2" ht="25">
       <c r="A5" s="47" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="B5" s="7"/>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="44" t="s">
-        <v>814</v>
+        <v>842</v>
       </c>
       <c r="B6" s="7"/>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="45" t="s">
-        <v>816</v>
+        <v>843</v>
       </c>
       <c r="B7" s="7"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="44" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="B8" s="7"/>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="45" t="s">
-        <v>828</v>
+        <v>844</v>
       </c>
       <c r="B9" s="7"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="45" t="s">
-        <v>818</v>
+        <v>845</v>
       </c>
       <c r="B10" s="7"/>
     </row>
@@ -34101,25 +34101,25 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="45" t="s">
-        <v>831</v>
+        <v>825</v>
       </c>
       <c r="B13" s="7"/>
     </row>
     <row r="14" spans="1:2" ht="25">
       <c r="A14" s="46" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="B14" s="7"/>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="45" t="s">
-        <v>817</v>
+        <v>840</v>
       </c>
       <c r="B15" s="7"/>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="44" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B16" s="7"/>
     </row>

</xml_diff>

<commit_message>
adds de-dupe users rake task. updates landing site template. updates user model
</commit_message>
<xml_diff>
--- a/public/templates/SmallPelagicLandingSite.template.xlsx
+++ b/public/templates/SmallPelagicLandingSite.template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <workbookProtection workbookPassword="C470" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="4760" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,14 @@
     <sheet name="Fishery Codes" sheetId="8" r:id="rId8"/>
     <sheet name="Desa Codes" sheetId="9" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="Desas">'Desa Codes'!$A$2:$A$16</definedName>
+    <definedName name="Fisheries">'Fishery Codes'!$A$2:$A$3</definedName>
+    <definedName name="Gears">'Gear Codes'!$A$2:$A$62</definedName>
+    <definedName name="Graticules">'Graticule Codes'!$A$2:$A$11</definedName>
+    <definedName name="Species">'Species Codes'!$A$2:$A$139</definedName>
+    <definedName name="Vessels">'Form A - Fleet'!$A$2:$A$51</definedName>
+  </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -2502,12 +2510,6 @@
     <t>No. vessels</t>
   </si>
   <si>
-    <t>Angantelo</t>
-  </si>
-  <si>
-    <t>Pesinggahan</t>
-  </si>
-  <si>
     <t>Dep. Date</t>
   </si>
   <si>
@@ -2562,10 +2564,16 @@
     <t>Bunutun</t>
   </si>
   <si>
-    <t>Jemelut</t>
-  </si>
-  <si>
     <t>Kusamba</t>
+  </si>
+  <si>
+    <t>Anantelo</t>
+  </si>
+  <si>
+    <t>Gemelut</t>
+  </si>
+  <si>
+    <t>Pessinggahan</t>
   </si>
 </sst>
 </file>
@@ -3844,7 +3852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3925,7 +3933,7 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation type="date" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the date on which this survey was conducted." sqref="B3">
       <formula1>40909</formula1>
       <formula2>55153</formula2>
@@ -3942,18 +3950,15 @@
       <formula1>0</formula1>
       <formula2>9999</formula2>
     </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a valid desa ID code. Please check the &quot;Desa Codes&quot; tab." sqref="B2">
+      <formula1>Desas</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a valid desa ID code. Please check the &quot;Desa Codes&quot; tab.">
-          <x14:formula1>
-            <xm:f>'Desa Codes'!A2:A1000</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a valid fishery ID code. Please check the &quot;Fishery Codes&quot; tab.">
           <x14:formula1>
             <xm:f>'Fishery Codes'!A2:A1000</xm:f>
@@ -4011,7 +4016,7 @@
         <v>820</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="J1" s="20" t="s">
         <v>13</v>
@@ -4020,7 +4025,7 @@
         <v>15</v>
       </c>
       <c r="L1" s="20" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="M1" s="20" t="s">
         <v>17</v>
@@ -4035,10 +4040,10 @@
         <v>23</v>
       </c>
       <c r="Q1" s="20" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="R1" s="20" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="S1" s="20" t="s">
         <v>805</v>
@@ -5430,7 +5435,7 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
-  <dataValidations count="16">
+  <dataValidations count="19">
     <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the volume of fuel in liters used during this trip (0-1000)." sqref="N2:N51">
       <formula1>0</formula1>
       <formula2>1000</formula2>
@@ -5490,32 +5495,19 @@
     <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a recognized code for the sea conditions. Permitted values are:_x000d__x000d_1: Calm_x000d_2: Moderate_x000d_3: Rough" sqref="R2:R51">
       <formula1>"1,2,3"</formula1>
     </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a valid graticule ID code. Please check the &quot;Graticule Codes&quot; tab." sqref="H2:H51">
+      <formula1>Graticules</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a valid gear ID code. Please check the &quot;Gear Codes&quot; tab." sqref="P2:P51">
+      <formula1>Gears</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a valid fish ID code. Please check the &quot;Fish Codes&quot; tab." sqref="S2:S51">
+      <formula1>Species</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a valid graticule ID code. Please check the &quot;Graticule Codes&quot; tab.">
-          <x14:formula1>
-            <xm:f>'Graticule Codes'!$A$2:$A$11</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H51</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a valid gear ID code. Please check the &quot;Gear Codes&quot; tab.">
-          <x14:formula1>
-            <xm:f>'Gear Codes'!$A$2:$A$62</xm:f>
-          </x14:formula1>
-          <xm:sqref>P2:P51</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a valid fish ID code. Please check the &quot;Fish Codes&quot; tab.">
-          <x14:formula1>
-            <xm:f>'Species Codes'!A1:A1000</xm:f>
-          </x14:formula1>
-          <xm:sqref>S2:S51</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
@@ -10149,7 +10141,7 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
-  <dataValidations count="2">
+  <dataValidations count="4">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="Enter a whole number representing the length of the fish in mm." sqref="D2:D500">
       <formula1>1</formula1>
       <formula2>10000</formula2>
@@ -10157,26 +10149,16 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check you entry" error="Enter the sampling factor._x000d__x000d_Enter 'c' for conspicuous fish sampled from the entire catch._x000d__x000d_Enter 's' for sampled fish from the first basket unloaded." sqref="E2:E500">
       <formula1>"c,s"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="Please select a species code from the list. See the 'species codes' tab for a complete list. " sqref="C2:C500">
+      <formula1>Species</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Enter a valid vessel number" error="Please check the tab 'Form A - Fleet' and enter a valid vessel ID number from which the catch was sampled" sqref="B2:B500">
+      <formula1>Vessels</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="Please select a species code from the list. See the 'species codes' tab for a complete list. ">
-          <x14:formula1>
-            <xm:f>'Species Codes'!$A$2:$A$139</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C500</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Enter a valid vessel number" error="Please check the tab 'Form A - Fleet' and enter a valid vessel ID number from which the catch was sampled">
-          <x14:formula1>
-            <xm:f>'Form A - Fleet'!$A$2:$A$51</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B500</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
@@ -10188,9 +10170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
@@ -11402,9 +11382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3451"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -33888,9 +33866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A11" sqref="A2:A11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
@@ -33905,52 +33881,52 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="30" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="30" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="30" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="30" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="30" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="30" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="30" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="30" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="30" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="30" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
     </row>
   </sheetData>
@@ -33969,9 +33945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
@@ -34017,9 +33991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
@@ -34035,7 +34007,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="44" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="B2" s="7"/>
     </row>
@@ -34047,7 +34019,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="44" t="s">
-        <v>824</v>
+        <v>843</v>
       </c>
       <c r="B4" s="7"/>
     </row>
@@ -34059,13 +34031,13 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="44" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="B6" s="7"/>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="45" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="B7" s="7"/>
     </row>
@@ -34083,7 +34055,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="45" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="B10" s="7"/>
     </row>
@@ -34101,7 +34073,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="45" t="s">
-        <v>825</v>
+        <v>845</v>
       </c>
       <c r="B13" s="7"/>
     </row>
@@ -34113,7 +34085,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="45" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="B15" s="7"/>
     </row>
@@ -34151,7 +34123,7 @@
       <c r="B23" s="7"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <sortState ref="A2:A16">
     <sortCondition ref="A2"/>
   </sortState>

</xml_diff>

<commit_message>
major update! Adds vessels, companies, protocols. Updates user and admin setting and security design. Adds google analytics. Adds jquery tour. Adds simple form presenters. Updates gems. Removes inherited reosurces.
</commit_message>
<xml_diff>
--- a/public/templates/SmallPelagicLandingSite.template.xlsx
+++ b/public/templates/SmallPelagicLandingSite.template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <workbookProtection workbookPassword="C470" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="4760" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="1" r:id="rId1"/>
@@ -5453,7 +5453,7 @@
     </dataValidation>
     <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter the total value of the catch in Rupia (0-100000000). Leave blank if not known." sqref="V2:V51">
       <formula1>0</formula1>
-      <formula2>100000000</formula2>
+      <formula2>1000000000</formula2>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check your entry" error="You must enter a valid engine type. Permitted values are:_x000d__x000d_OB : Outboard_x000d_IB : Inboard_x000d_LT : Longtail" sqref="E2:E51">
       <formula1>"OB,LT,IB"</formula1>

</xml_diff>